<commit_message>
Add Import Drivers Sample File
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportDriversSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportDriversSampleFile.xlsx
@@ -5,34 +5,30 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\OneDrive\Desktop\Trucks &amp; Drivers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Trucks &amp; Drivers\Driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D862F3AA-7993-4D69-9E8D-C2D9F66B5FB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Ong6jC8xobpEciVYsibVv/DAniA6JWo6M+aAnrjiQaPdKqw3r6bjhQfzDQveVZh5q/vHi8AacO59cPkM8TpWfQ==" workbookSaltValue="xdqeOWlJGzkQUPAY86HjQA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A467407-B34F-448F-A79D-664438C51CF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2850" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
-  <si>
-    <t>Surname*</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Name*</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ID/Iqama/ NO*</t>
   </si>
   <si>
-    <t>Phone Number*</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Email Address</t>
   </si>
   <si>
     <t>Occupation Card NO</t>
@@ -53,27 +49,26 @@
     <t>Driving License Expiry Date(Hijri)</t>
   </si>
   <si>
-    <t>testImport</t>
-  </si>
-  <si>
-    <t>testImport2</t>
-  </si>
-  <si>
-    <t>30/4/1442</t>
-  </si>
-  <si>
-    <t>26/11/2020</t>
+    <t xml:space="preserve"> First Name*</t>
+  </si>
+  <si>
+    <t>Last Name*</t>
+  </si>
+  <si>
+    <t>Date of Birth(Hijri)</t>
+  </si>
+  <si>
+    <t>Date of Birth(Gregorian)</t>
+  </si>
+  <si>
+    <t>Mobile Number*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-1170000]B2dd/mm/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
-  </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -101,30 +96,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,23 +124,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,135 +444,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485524A3-FF2C-429E-973D-68DAEE8DA526}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="15.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="4" width="15.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.08984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>900000002</v>
-      </c>
-      <c r="D2" s="2">
-        <v>900000002</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2">
-        <v>900000002</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2">
-        <v>900000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
-        <v>900000003</v>
-      </c>
-      <c r="D3" s="2">
-        <v>900000003</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2">
-        <v>900000003</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="2">
-        <v>900000003</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations xWindow="678" yWindow="260" count="13">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver ID/Iqama number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="D1 D4:D1048576" xr:uid="{1074CB78-DFC4-4B0A-A0E6-C4419DC127EE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the driver ID/Iqama,(Note: the date is mandatory, and you can enter the date in Gregorian or Hijri, in this field please use Gregorian date: DD/MM/YYYY )" sqref="F1 F4:F1048576" xr:uid="{4BA3844E-0126-4DD3-8C5A-476B5060D44F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver license number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="G4:G1048576 G1" xr:uid="{321BD3F3-82FD-44E7-A591-2C8E5BC5DF31}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the driver licens, (Note: the date is mandatory, and you can enter the date in Gregorian or Hijri, in this field please use Gregorian date: DD/MM/YYYY )" sqref="I1 I4:I1048576" xr:uid="{D071BF54-445B-4EB5-A4DC-A884C5FF2DEC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver first name (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="A1:A1048576" xr:uid="{D0B5C4DB-823F-412A-BF37-81BBFEF7432C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver mobile number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="C1:C1048576 D2:D3 J2:J3 G2:G3" xr:uid="{3A9285A5-B5DB-464B-A486-F82E7497D9B0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver last name (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="B2:B1048576" xr:uid="{81683B50-66DC-4C78-A4CE-7BFD79206093}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the occupation card number " sqref="J1 J4:J1048576" xr:uid="{DD119572-1393-4E3C-A44C-DEA4BA898E70}"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="9L29B6uEWsKsHrbB2OEX6RyTgEGnPgOMfKbZZApimSXJIVtOYim+aRMZdeDlAzla9X9MX4qyD2kUx67U80IlTw==" saltValue="qy1x51asrubCmmK88GYeng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="13">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver email" sqref="D1" xr:uid="{BCBA06BC-1B6E-4821-9149-56B85CE5D524}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver ID/Iqama number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="G1" xr:uid="{1074CB78-DFC4-4B0A-A0E6-C4419DC127EE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver license number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="J1" xr:uid="{321BD3F3-82FD-44E7-A591-2C8E5BC5DF31}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Driving License expiration date, either Hijri or Gregorian dates (Note: in this field please use Gregorian date: DD/MM/YYYY )" sqref="L1" xr:uid="{D071BF54-445B-4EB5-A4DC-A884C5FF2DEC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver first name (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="A1" xr:uid="{D0B5C4DB-823F-412A-BF37-81BBFEF7432C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver mobile number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="C1" xr:uid="{3A9285A5-B5DB-464B-A486-F82E7497D9B0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the occupation card number " sqref="M1" xr:uid="{DD119572-1393-4E3C-A44C-DEA4BA898E70}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver last name_x000a_(Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="B1" xr:uid="{9F6E3987-549B-4E8B-AFBF-10E95B72D532}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the driver ID/Iqama, (Note: the date is mandatory, and you can enter the date in Gregorian or Hijri, in this field please use Hijri, date: DD/MM/YYYY )" sqref="E1 E4:E1048576" xr:uid="{742D905C-6D82-4A25-A7A7-44D5994C15CD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add the expiration date for the driver licens, (Note: the date is mandatory, and you can enter the date in Gregorian or Hijri, in this field please use Hijri, date: DD/MM/YYYY )" sqref="H1 H4:H1048576" xr:uid="{525E21A9-190B-48D5-AD17-66FAC0D77DC2}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, you can enter the date in Gregorian or Hijri, in this field please use Hijri date: DD/MM/YYYY (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="E2:E3 H2:H3" xr:uid="{5C0340A2-E120-4645-A97A-5EB9E5B5B9C0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Istimara expiration date, you can enter the date in Gregorian or Hijri, in this field please use Gregorian date: DD/MM/YYYY (Note: this is a mandatory field, your file will be rejectd if this field is empty)" sqref="F2:F3 I2:I3" xr:uid="{A5CBD075-51A2-42FD-9BE9-85E69DC8DF9C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add ID/Iqama expiration date, either Hijri or Gregorian dates (Note: in this field please use Gregorian date: DD/MM/YYYY )" sqref="I1" xr:uid="{742D905C-6D82-4A25-A7A7-44D5994C15CD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add Driving License expiration date, either Hijri or Gregorian dates (Note: in this field please use Hijri date: DD/MM/YYYY )" sqref="K1" xr:uid="{525E21A9-190B-48D5-AD17-66FAC0D77DC2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add ID/Iqama expiration date, either Hijri or Gregorian dates (Note: in this field please use Hijri date: DD/MM/YYYY )" sqref="H1" xr:uid="{9F7185B6-0CF9-400D-8801-AA33065D20BA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver birth date either Hijri or Gregorian dates (Note: in this field please use Gregorian date: DD/MM/YYYY)" sqref="F1" xr:uid="{B37AB55A-1165-40BE-AE49-51B9680CDF09}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver birth date either Hijri or Gregorian dates (Note: in this field please use Hijri date: DD/MM/YYYY )" sqref="E1" xr:uid="{598FDA7C-E931-4FA3-AB53-8D78A7F46BAE}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add multi lingual import from excel
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportDriversSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportDriversSampleFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Trucks &amp; Drivers\Driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\source\tachyon-core\angular\src\assets\sampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A467407-B34F-448F-A79D-664438C51CF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD42782-46FE-4705-A2A0-23FF73F594F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25974" yWindow="-109" windowWidth="21954" windowHeight="11982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -68,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -446,25 +446,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485524A3-FF2C-429E-973D-68DAEE8DA526}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="11.55"/>
   <cols>
-    <col min="1" max="4" width="15.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.08984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="15.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="31.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="2"/>
+    <col min="10" max="10" width="32.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -505,13 +505,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9L29B6uEWsKsHrbB2OEX6RyTgEGnPgOMfKbZZApimSXJIVtOYim+aRMZdeDlAzla9X9MX4qyD2kUx67U80IlTw==" saltValue="qy1x51asrubCmmK88GYeng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver email" sqref="D1" xr:uid="{BCBA06BC-1B6E-4821-9149-56B85CE5D524}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please add driver ID/Iqama number (Note: this is a mandatory field, your file will be rejected if this field is empty)" sqref="G1" xr:uid="{1074CB78-DFC4-4B0A-A0E6-C4419DC127EE}"/>

</xml_diff>

<commit_message>
Change default Arabic culture to ar-EG
This will force use Gregorian calendar in Arabic language
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/ImportDriversSampleFile.xlsx
+++ b/angular/src/assets/sampleFiles/ImportDriversSampleFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\source\tachyon-core\angular\src\assets\sampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD42782-46FE-4705-A2A0-23FF73F594F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66CBC85-0AA7-4487-9DDA-0E4BC9A87C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="21954" windowHeight="11982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2418" windowWidth="26219" windowHeight="8110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -118,17 +118,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,22 +446,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485524A3-FF2C-429E-973D-68DAEE8DA526}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="I128" sqref="I128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="11.55"/>
   <cols>
-    <col min="1" max="4" width="15.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="31.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.75" style="2"/>
+    <col min="1" max="4" width="15.625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="27.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="31.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.75" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -483,7 +483,7 @@
       <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -492,21 +492,21 @@
       <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>